<commit_message>
Comentários, dúvidas e sugestões sobre os artefatos iniciais
</commit_message>
<xml_diff>
--- a/Lista Inicial de Requisitos 2.xlsx
+++ b/Lista Inicial de Requisitos 2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="90" windowWidth="14355" windowHeight="4680"/>
@@ -11,12 +11,12 @@
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="58">
   <si>
     <t>NUM</t>
   </si>
@@ -63,15 +63,9 @@
     <t>UC006</t>
   </si>
   <si>
-    <t>Manter usuário</t>
-  </si>
-  <si>
     <t>Manter funionário</t>
   </si>
   <si>
-    <t>Cadastrar calendário</t>
-  </si>
-  <si>
     <t>O cliente consulta boleto (no ambiente cliente)</t>
   </si>
   <si>
@@ -138,9 +132,6 @@
     <t>Atores</t>
   </si>
   <si>
-    <t>Manter funcionário</t>
-  </si>
-  <si>
     <t>Gerente, Funcionário</t>
   </si>
   <si>
@@ -153,20 +144,59 @@
     <t>Upload Boleto</t>
   </si>
   <si>
-    <t>Manter Cliente</t>
-  </si>
-  <si>
     <t>Cliente</t>
   </si>
   <si>
     <t>Sistema</t>
+  </si>
+  <si>
+    <t>Manter cadastro dos usuários do sistema.</t>
+  </si>
+  <si>
+    <t>COMENTÁRIOS</t>
+  </si>
+  <si>
+    <t>Manter os usuários do sistema tem relação com a permissão do acesso de pessoas ao sistema, sejam funcionários, clientes, etc. Isso é diferente de manter um cadastro dos clientes que vão usar o sistema e que pagam os impostos. Nesse caso seriam dois casos de uso diferentes (Manter Usuários e Manter Clientes). Além disso, aqui aparece um ator Gerente que não foi citado no texto. Quem é esse gerente e o que ele faz no sistema?</t>
+  </si>
+  <si>
+    <t>Manter Clientes</t>
+  </si>
+  <si>
+    <t>Manter Funcionários</t>
+  </si>
+  <si>
+    <t>Existem dois tipos de funcionários (Gerente e Funcionário)?. É o que parece pela leitura.</t>
+  </si>
+  <si>
+    <t>Cadastrar calendário, Manter Clientes</t>
+  </si>
+  <si>
+    <t>Não foram mencionados nem explicados o que ou quais seriam esses três tipos de calendário. Coloquei a associação com o caso de uso Manter Clientes pois além de se cadastrar um calendário deve haver alguma funcionalidade para associar um cliente a um calendário, provavelmente durante o cadastro do cliente.</t>
+  </si>
+  <si>
+    <t>Como já comentei na descrição, o boleto está surgindo do nada, quando na verdade deveria ser gerado a partir das informações contidas no cadastro do cliente e no cadastro de impostos que deveria existir no sistema (mas não existe).</t>
+  </si>
+  <si>
+    <t>Neste caso seria "Consultar Histórico de Boletos de um Cliente" e não "Registrar Histórico".</t>
+  </si>
+  <si>
+    <t>Os demais atores (Gerente e Funcionário) não possuem login?</t>
+  </si>
+  <si>
+    <t>Acho mais apropriado o cliente consultar sua agenda de vencimentos e a partir daí poder consultar e/ou baixar os boletos correspondentes às obrigações que ele tem para pagar. Assim um nome de UC mais apropriado seria "Consultar Agenda de Vencimentos" ou "Consultar Obrigações a Pagar" ou algo parecido.</t>
+  </si>
+  <si>
+    <t>Vale a mesma observação já feita anteriormente. Se o sistema mantém um cadastro com os vencimentos dos impostos e os clientes estão associados a esses impostos, então não vejo necessidade de que um funcionário faça um "upload" de boleto. Acho mais lógico que o cliente faça a consulta de sua obrigações e a partir daí o sistema verifica automaticamente o que ele tem para pagar de acordo com o seu cadastro e com os vencimentos dos impostos. Em seguida, o cliente pode gerar e baixar os boletos que desejar.</t>
+  </si>
+  <si>
+    <t>FAVOR DEIXAR APENAS UMA VERSÃO DE CADA ARQUIVO, OU SEJA, AQUELA QUE ESTÁ VALENDO, POIS SE EXISTE MAIS DE UMA PODE HAVER CONFUSÃO, INCLUSIVE EU POSSO ESTAR FAZENDO COMENTÁRIOS NA VERSÃO ERRADA.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,7 +227,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -220,11 +250,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -235,6 +276,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -324,7 +378,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -359,7 +412,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -535,22 +587,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="38.42578125" customWidth="1"/>
     <col min="3" max="3" width="8.42578125" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" customWidth="1"/>
     <col min="5" max="5" width="32.5703125" customWidth="1"/>
+    <col min="6" max="6" width="45.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -564,227 +617,259 @@
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="150">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>15</v>
+      <c r="B3" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>16</v>
+      <c r="B4" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="105">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>19</v>
+      <c r="B5" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="75">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>23</v>
+      <c r="B6" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="105">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>18</v>
+      <c r="B7" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="38.25" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>36</v>
+      <c r="B8" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="180">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30">
+      <c r="A11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30">
+      <c r="A12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="D12" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="1"/>
       <c r="D13" s="2"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="C14" s="1"/>
       <c r="D14" s="2"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="C15" s="1"/>
       <c r="D15" s="2"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="1"/>
       <c r="D16" s="2"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="1"/>
       <c r="D17" s="2"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="C18" s="1"/>
       <c r="D18" s="2"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="C19" s="1"/>
       <c r="D19" s="2"/>
       <c r="E19" s="1"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="B23" s="8" t="s">
+        <v>57</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -793,24 +878,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>